<commit_message>
Added GUI resources and source code
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="122">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -143,10 +143,10 @@
     <t xml:space="preserve">Small</t>
   </si>
   <si>
-    <t xml:space="preserve">labels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NotoSans-Regular.ttf</t>
+    <t xml:space="preserve">EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789 :APM</t>
   </si>
   <si>
     <t xml:space="preserve">-., 0123456789</t>
@@ -155,22 +155,232 @@
     <t xml:space="preserve">SingleUseId1</t>
   </si>
   <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TextId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Right</t>
   </si>
   <si>
-    <t xml:space="preserve">LTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Left</t>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjust screen brightness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change time and date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">⇩</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">⇧</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">state: recording</t>
+  </si>
+  <si>
+    <t xml:space="preserve">state: idle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789 :APM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt; %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId51</t>
   </si>
 </sst>
 </file>
@@ -1398,13 +1608,13 @@
     </row>
     <row r="4" spans="2:16">
       <c r="B4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1413,7 +1623,9 @@
         <v>17</v>
       </c>
       <c r="G4"/>
-      <c r="H4"/>
+      <c r="H4" t="s">
+        <v>118</v>
+      </c>
       <c r="I4"/>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
@@ -1433,6 +1645,23 @@
       </c>
     </row>
     <row r="5" spans="2:16">
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="L5" s="7" t="s">
@@ -1450,6 +1679,25 @@
       <c r="P5" s="10"/>
     </row>
     <row r="6" spans="2:16">
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
       <c r="I6"/>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
@@ -1467,6 +1715,25 @@
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16">
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
       <c r="L7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1484,6 +1751,25 @@
       </c>
     </row>
     <row r="8" spans="2:16">
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
       <c r="L8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1594,7 +1880,7 @@
         <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4">
@@ -1602,7 +1888,7 @@
         <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
         <v>46</v>
@@ -1619,7 +1905,7 @@
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
         <v>51</v>
@@ -1628,9 +1914,343 @@
         <v>47</v>
       </c>
       <c r="F5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
         <v>49</v>
       </c>
     </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added custom button icons
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="144">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -381,6 +381,72 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pause testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId65</t>
   </si>
 </sst>
 </file>
@@ -1785,6 +1851,25 @@
       <c r="P8" s="10"/>
     </row>
     <row r="9" spans="2:16">
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
       <c r="L9" s="11" t="s">
         <v>6</v>
       </c>
@@ -1953,10 +2038,10 @@
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
         <v>51</v>
@@ -1965,66 +2050,66 @@
         <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
         <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
         <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
         <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
@@ -2033,15 +2118,15 @@
         <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D13" t="s">
         <v>51</v>
@@ -2050,29 +2135,29 @@
         <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
         <v>82</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
         <v>82</v>
@@ -2084,12 +2169,12 @@
         <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C16" t="s">
         <v>82</v>
@@ -2101,12 +2186,12 @@
         <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
         <v>82</v>
@@ -2118,49 +2203,49 @@
         <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
         <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
         <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
         <v>46</v>
@@ -2169,32 +2254,32 @@
         <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
         <v>47</v>
       </c>
       <c r="F21" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="D22" t="s">
         <v>51</v>
@@ -2203,12 +2288,12 @@
         <v>47</v>
       </c>
       <c r="F22" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C23" t="s">
         <v>38</v>
@@ -2220,19 +2305,179 @@
         <v>47</v>
       </c>
       <c r="F23" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>138</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" t="s">
+        <v>137</v>
+      </c>
+    </row>
     <row r="34"/>
     <row r="35"/>
     <row r="36"/>

</xml_diff>

<commit_message>
Added scrolling text output for testing
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2845" uniqueCount="146">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -447,6 +447,12 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,a-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00-0xFF</t>
   </si>
 </sst>
 </file>
@@ -1692,7 +1698,9 @@
       <c r="H4" t="s">
         <v>118</v>
       </c>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>145</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1728,7 +1736,9 @@
       </c>
       <c r="G5"/>
       <c r="H5"/>
-      <c r="I5"/>
+      <c r="I5" t="s">
+        <v>145</v>
+      </c>
       <c r="J5"/>
       <c r="L5" s="7" t="s">
         <v>1</v>
@@ -1764,7 +1774,9 @@
       <c r="H6" t="s">
         <v>44</v>
       </c>
-      <c r="I6"/>
+      <c r="I6" t="s">
+        <v>145</v>
+      </c>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
         <v>2</v>
@@ -1798,7 +1810,9 @@
       </c>
       <c r="G7"/>
       <c r="H7"/>
-      <c r="I7"/>
+      <c r="I7" t="s">
+        <v>145</v>
+      </c>
       <c r="J7"/>
       <c r="L7" s="7" t="s">
         <v>7</v>
@@ -1834,7 +1848,9 @@
       </c>
       <c r="G8"/>
       <c r="H8"/>
-      <c r="I8"/>
+      <c r="I8" t="s">
+        <v>145</v>
+      </c>
       <c r="J8"/>
       <c r="L8" s="7" t="s">
         <v>8</v>
@@ -1868,7 +1884,9 @@
       </c>
       <c r="G9"/>
       <c r="H9"/>
-      <c r="I9"/>
+      <c r="I9" t="s">
+        <v>145</v>
+      </c>
       <c r="J9"/>
       <c r="L9" s="11" t="s">
         <v>6</v>

</xml_diff>